<commit_message>
Commited after query changes
</commit_message>
<xml_diff>
--- a/ocms/src/test/resources/TestData/OCMAgentAuxReportData.xlsx
+++ b/ocms/src/test/resources/TestData/OCMAgentAuxReportData.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21929"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E91A74F6-4626-4FA7-BA61-6F8A82B3EF85}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3631AF23-50E0-4107-99CA-C719677CAF40}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10560" firstSheet="5" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -111,11 +111,17 @@
     <t>Query</t>
   </si>
   <si>
-    <t>SELECT M.[AgentID],A.[AgentName],M.[AuxName],M.[AuxCode],
+    <t>17-04-2020 00:00:00</t>
+  </si>
+  <si>
+    <t>20-04-2020 00:00:00</t>
+  </si>
+  <si>
+    <t>SELECT M.[AgentID],A.[AgentName],A.[TeamName],A.[SupervisorName],M.[AuxName],M.[AuxCode],
 CONVERT(char(8),DATEADD(second,sum((DATEPART(hh,CONVERT(varchar, DATEADD(ms, AuxTime* 1000, 0), 108))*3600)+
 (DATEPART(mi,CONVERT(varchar, DATEADD(ms, AuxTime* 1000, 0), 108))*60)+
 DATEPART(ss,CONVERT(varchar, DATEADD(ms, AuxTime* 1000, 0), 108))),0),108)
-as [AuxTime],A.[TeamName],A.[SupervisorName] from
+as [AuxTime] from
 (SELECT Distinct T1.AgentID,ISNULL(A.[Username],' ')  AS AgentName,T1.[Status] AS AuxName,
 isnull(convert(varchar,C.[value]),' ') AS AuxCode,
 isnull((DATEDIFF(SECOND,convert(datetime,stuff(stuff(stuff(T1.[TimeStamp], 9, 0, ' '), 12, 0, ':'), 15, 0, ':')),
@@ -131,12 +137,6 @@
 AND M.[AuxName] NOT IN ('Login','Logout','Default','Skillaux')
 group by M.[AgentID],A.[AgentName],[AuxName],M.[AuxCode],A.[TeamName],A.[SupervisorName] 
 order by M.AgentID, M.AuxName</t>
-  </si>
-  <si>
-    <t>17-04-2020 00:00:00</t>
-  </si>
-  <si>
-    <t>20-04-2020 00:00:00</t>
   </si>
 </sst>
 </file>
@@ -986,7 +986,7 @@
   <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B2" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1028,13 +1028,13 @@
         <v>6</v>
       </c>
       <c r="D2" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="E2" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="E2" s="8" t="s">
+      <c r="F2" s="9" t="s">
         <v>29</v>
-      </c>
-      <c r="F2" s="9" t="s">
-        <v>27</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Committed on 22nd April
</commit_message>
<xml_diff>
--- a/ocms/src/test/resources/TestData/OCMAgentAuxReportData.xlsx
+++ b/ocms/src/test/resources/TestData/OCMAgentAuxReportData.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21929"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3631AF23-50E0-4107-99CA-C719677CAF40}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7CDEF11E-36B1-41DF-8D94-1C8C448BD394}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10560" firstSheet="5" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -117,7 +117,7 @@
     <t>20-04-2020 00:00:00</t>
   </si>
   <si>
-    <t>SELECT M.[AgentID],A.[AgentName],A.[TeamName],A.[SupervisorName],M.[AuxName],M.[AuxCode],
+    <t>SELECT M.[AgentID] as [Agent ID],A.[AgentName] as [Agent Name],A.[TeamName] as [Team Name],A.[SupervisorName] as [Supervisor Name],M.[AuxName],M.[AuxCode],
 CONVERT(char(8),DATEADD(second,sum((DATEPART(hh,CONVERT(varchar, DATEADD(ms, AuxTime* 1000, 0), 108))*3600)+
 (DATEPART(mi,CONVERT(varchar, DATEADD(ms, AuxTime* 1000, 0), 108))*60)+
 DATEPART(ss,CONVERT(varchar, DATEADD(ms, AuxTime* 1000, 0), 108))),0),108)
@@ -136,7 +136,7 @@
 INNER JOIN fn_AgentHierarchy('na','1','1') A ON A.[AgentId]=M.[AgentID] 
 AND M.[AuxName] NOT IN ('Login','Logout','Default','Skillaux')
 group by M.[AgentID],A.[AgentName],[AuxName],M.[AuxCode],A.[TeamName],A.[SupervisorName] 
-order by M.AgentID, M.AuxName</t>
+order by M.AgentID,A.TeamName,M.AuxName</t>
   </si>
 </sst>
 </file>
@@ -986,7 +986,7 @@
   <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B2" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>